<commit_message>
lớp tập huấn danh sách giáo viên, import
</commit_message>
<xml_diff>
--- a/public/download/DS_TAP_HUAN.xlsx
+++ b/public/download/DS_TAP_HUAN.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO-FPT\Desktop\Hiepphat\Web\hiep-phat\public\download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B673CE8D-2B57-4D44-80DC-5D28C8BE17CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BD92EA-962C-44F9-A516-253ACB445D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -264,12 +264,27 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -278,21 +293,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -740,22 +740,22 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="A4" sqref="A4:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="7" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="7.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" style="1" customWidth="1"/>
     <col min="10" max="10" width="7.88671875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="15.77734375" style="5" customWidth="1"/>
     <col min="12" max="12" width="7.88671875" style="1" customWidth="1"/>
     <col min="13" max="13" width="9.44140625" style="1" customWidth="1"/>
     <col min="14" max="14" width="13.88671875" style="1" customWidth="1"/>
@@ -767,148 +767,148 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
       <c r="E1" s="8"/>
       <c r="F1" s="7"/>
       <c r="G1" s="8"/>
       <c r="H1" s="7"/>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
     </row>
     <row r="2" spans="1:15" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
       <c r="E2" s="8"/>
       <c r="F2" s="7"/>
       <c r="G2" s="8"/>
       <c r="H2" s="7"/>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
     </row>
     <row r="3" spans="1:15" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
     </row>
     <row r="4" spans="1:15" s="3" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
     </row>
     <row r="5" spans="1:15" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
     </row>
     <row r="6" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16" t="s">
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="17" t="s">
+      <c r="K6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="16" t="s">
+      <c r="L6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="19" t="s">
+      <c r="M6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="N6" s="16" t="s">
+      <c r="N6" s="11" t="s">
         <v>20</v>
       </c>
       <c r="O6" s="6"/>
     </row>
     <row r="7" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="16"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="11"/>
       <c r="G7" s="9" t="s">
         <v>9</v>
       </c>
@@ -918,37 +918,49 @@
       <c r="I7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="16"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="16"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="11"/>
       <c r="O7" s="6"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
     </row>
     <row r="12" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <autoFilter ref="N1:N10" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <mergeCells count="20">
+    <mergeCell ref="H8:M8"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="I1:M1"/>
+    <mergeCell ref="I2:M2"/>
+    <mergeCell ref="B6:C7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
     <mergeCell ref="N6:N7"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="D6:D7"/>
@@ -957,18 +969,6 @@
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="M6:M7"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="I1:M1"/>
-    <mergeCell ref="I2:M2"/>
-    <mergeCell ref="B6:C7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="H8:M8"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="A5:M5"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.31496062992125984" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>